<commit_message>
initial commit of this branch
</commit_message>
<xml_diff>
--- a/etc/Timeline for migrating Gotesco to Accupay.xlsx
+++ b/etc/Timeline for migrating Gotesco to Accupay.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545749B2-581C-45B8-9136-E8DD0C8EEA01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="499" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>identify which Gotesco payroll requirements are not yet supported by AccuPay</t>
   </si>
@@ -54,16 +55,19 @@
   </si>
   <si>
     <t>GOTESCO FUNCTIONALITY NOT YET IN ACCUPAY</t>
+  </si>
+  <si>
+    <t>employee files its own leave, ot, or ob</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="@\.\)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,11 +137,19 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -184,7 +196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,9 +228,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,6 +280,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,7 +473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -435,13 +483,13 @@
       <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="95" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
@@ -449,7 +497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -460,7 +508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -471,7 +519,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -489,41 +537,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>